<commit_message>
FINAL VERSION NO CHANGES
</commit_message>
<xml_diff>
--- a/coordinates.xlsx
+++ b/coordinates.xlsx
@@ -5,22 +5,35 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shami\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonathan\Desktop\oschack\room-finder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF2B8314-C7A9-4D95-B58A-BE5E16846BB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6213662-8A1C-498B-B4DA-0685C22B0003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11438" yWindow="0" windowWidth="11684" windowHeight="13763" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="450" windowWidth="14400" windowHeight="15750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="408">
   <si>
     <t>prefix</t>
   </si>
@@ -1238,6 +1251,12 @@
   </si>
   <si>
     <t>Honey Bee Research and Extension Lab</t>
+  </si>
+  <si>
+    <t>SHK</t>
+  </si>
+  <si>
+    <t>Shrek's Swamp</t>
   </si>
 </sst>
 </file>
@@ -1571,19 +1590,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D102"/>
+  <dimension ref="A1:D103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
       <selection activeCell="D102" sqref="D102"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="18.53125" customWidth="1"/>
-    <col min="4" max="4" width="27.19921875" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1597,7 +1616,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1611,7 +1630,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1625,7 +1644,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1639,7 +1658,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -1653,7 +1672,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -1667,7 +1686,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1681,7 +1700,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -1695,7 +1714,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -1709,7 +1728,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -1723,7 +1742,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -1737,7 +1756,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -1751,7 +1770,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -1765,7 +1784,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>39</v>
       </c>
@@ -1779,7 +1798,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -1793,7 +1812,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>45</v>
       </c>
@@ -1807,7 +1826,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>48</v>
       </c>
@@ -1821,7 +1840,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>51</v>
       </c>
@@ -1835,7 +1854,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>54</v>
       </c>
@@ -1849,7 +1868,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>57</v>
       </c>
@@ -1863,7 +1882,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>60</v>
       </c>
@@ -1877,7 +1896,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>63</v>
       </c>
@@ -1891,7 +1910,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>66</v>
       </c>
@@ -1905,7 +1924,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>69</v>
       </c>
@@ -1919,7 +1938,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>72</v>
       </c>
@@ -1933,7 +1952,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>75</v>
       </c>
@@ -1947,7 +1966,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>78</v>
       </c>
@@ -1961,7 +1980,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>81</v>
       </c>
@@ -1975,7 +1994,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>84</v>
       </c>
@@ -1989,7 +2008,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>87</v>
       </c>
@@ -2003,7 +2022,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>90</v>
       </c>
@@ -2017,7 +2036,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>93</v>
       </c>
@@ -2031,7 +2050,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>96</v>
       </c>
@@ -2045,7 +2064,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>99</v>
       </c>
@@ -2059,7 +2078,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>102</v>
       </c>
@@ -2073,7 +2092,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>105</v>
       </c>
@@ -2087,7 +2106,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>108</v>
       </c>
@@ -2101,7 +2120,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>111</v>
       </c>
@@ -2115,7 +2134,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>114</v>
       </c>
@@ -2129,7 +2148,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>117</v>
       </c>
@@ -2143,7 +2162,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>120</v>
       </c>
@@ -2157,7 +2176,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>123</v>
       </c>
@@ -2171,7 +2190,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>126</v>
       </c>
@@ -2185,7 +2204,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>129</v>
       </c>
@@ -2199,7 +2218,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>132</v>
       </c>
@@ -2213,7 +2232,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>135</v>
       </c>
@@ -2227,7 +2246,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>138</v>
       </c>
@@ -2241,7 +2260,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>141</v>
       </c>
@@ -2255,7 +2274,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>144</v>
       </c>
@@ -2269,7 +2288,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>147</v>
       </c>
@@ -2283,7 +2302,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>150</v>
       </c>
@@ -2297,7 +2316,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>153</v>
       </c>
@@ -2311,7 +2330,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>156</v>
       </c>
@@ -2325,7 +2344,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>159</v>
       </c>
@@ -2339,7 +2358,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>162</v>
       </c>
@@ -2353,7 +2372,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>165</v>
       </c>
@@ -2367,7 +2386,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>168</v>
       </c>
@@ -2381,7 +2400,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>171</v>
       </c>
@@ -2395,7 +2414,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>174</v>
       </c>
@@ -2409,7 +2428,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>177</v>
       </c>
@@ -2423,7 +2442,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>180</v>
       </c>
@@ -2437,7 +2456,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>183</v>
       </c>
@@ -2451,7 +2470,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>186</v>
       </c>
@@ -2465,7 +2484,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>189</v>
       </c>
@@ -2479,7 +2498,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>192</v>
       </c>
@@ -2493,7 +2512,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>195</v>
       </c>
@@ -2507,7 +2526,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>198</v>
       </c>
@@ -2521,7 +2540,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>201</v>
       </c>
@@ -2535,7 +2554,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>204</v>
       </c>
@@ -2549,7 +2568,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>207</v>
       </c>
@@ -2563,7 +2582,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>210</v>
       </c>
@@ -2577,7 +2596,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>213</v>
       </c>
@@ -2591,7 +2610,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>216</v>
       </c>
@@ -2605,7 +2624,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>219</v>
       </c>
@@ -2619,7 +2638,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>222</v>
       </c>
@@ -2633,7 +2652,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>225</v>
       </c>
@@ -2647,7 +2666,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>228</v>
       </c>
@@ -2661,7 +2680,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>231</v>
       </c>
@@ -2675,7 +2694,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>234</v>
       </c>
@@ -2689,7 +2708,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>237</v>
       </c>
@@ -2703,7 +2722,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>240</v>
       </c>
@@ -2717,7 +2736,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>243</v>
       </c>
@@ -2731,7 +2750,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>246</v>
       </c>
@@ -2745,7 +2764,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>249</v>
       </c>
@@ -2759,7 +2778,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>252</v>
       </c>
@@ -2773,7 +2792,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>255</v>
       </c>
@@ -2787,7 +2806,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>258</v>
       </c>
@@ -2801,7 +2820,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>261</v>
       </c>
@@ -2815,7 +2834,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>264</v>
       </c>
@@ -2829,7 +2848,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>267</v>
       </c>
@@ -2843,7 +2862,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>270</v>
       </c>
@@ -2857,7 +2876,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>273</v>
       </c>
@@ -2871,7 +2890,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>276</v>
       </c>
@@ -2885,7 +2904,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>279</v>
       </c>
@@ -2899,7 +2918,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>280</v>
       </c>
@@ -2913,7 +2932,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>283</v>
       </c>
@@ -2927,7 +2946,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>286</v>
       </c>
@@ -2941,7 +2960,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>289</v>
       </c>
@@ -2955,7 +2974,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>292</v>
       </c>
@@ -2969,7 +2988,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>295</v>
       </c>
@@ -2983,7 +3002,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>298</v>
       </c>
@@ -2997,7 +3016,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>301</v>
       </c>
@@ -3009,6 +3028,20 @@
       </c>
       <c r="D102" t="s">
         <v>404</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>406</v>
+      </c>
+      <c r="B103">
+        <v>69</v>
+      </c>
+      <c r="C103">
+        <v>69</v>
+      </c>
+      <c r="D103" t="s">
+        <v>407</v>
       </c>
     </row>
   </sheetData>

</xml_diff>